<commit_message>
Bot mandando e marcando no grupo(So falta acha no grupo)
</commit_message>
<xml_diff>
--- a/planilha_excel/Modelo.xlsx
+++ b/planilha_excel/Modelo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas Georgini\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas Loures\Desktop\BOTZAP\planilha_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90C9D219-2ECD-474D-8051-35D712208AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C0B922-2C40-453C-B7D5-9705C74B3EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{D637EA93-E164-41D0-97BA-2000602AB2C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D637EA93-E164-41D0-97BA-2000602AB2C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="2" r:id="rId1"/>
@@ -26,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -91,10 +89,10 @@
     <t>Wellington Freitas</t>
   </si>
   <si>
-    <t>JOSE MARIA JOAO</t>
-  </si>
-  <si>
-    <t>MARIA JOAQUINA JOAO</t>
+    <t>Newzinho</t>
+  </si>
+  <si>
+    <t>Matozinhos</t>
   </si>
 </sst>
 </file>
@@ -505,7 +503,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>